<commit_message>
Removed doc-pageheader and doc-pagefooter from tests results
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB aria test results.xlsx
+++ b/dpub-aria-testing/test-results/DPUB aria test results.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6F2D182-71A4-E94F-A3B5-3D0CBF4005E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="30400" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
   <si>
     <t>DPUB aria roles</t>
   </si>
@@ -112,12 +111,6 @@
     <t>doc-pagelist</t>
   </si>
   <si>
-    <t>doc-pagefooter</t>
-  </si>
-  <si>
-    <t>doc-pageheader</t>
-  </si>
-  <si>
     <t>doc-part</t>
   </si>
   <si>
@@ -184,9 +177,6 @@
     <t>separator (computed)</t>
   </si>
   <si>
-    <t>no role associated</t>
-  </si>
-  <si>
     <t>Role with Chrome / Mac</t>
   </si>
   <si>
@@ -221,18 +211,12 @@
   </si>
   <si>
     <t>"Horizontal separator, title has P1"</t>
-  </si>
-  <si>
-    <t>doc-pagefooter (strange this were mapped)</t>
-  </si>
-  <si>
-    <t>doc-pageheader (strange this were mapped)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,7 +308,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,26 +341,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,23 +376,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -601,71 +551,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.6328125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="35.5" customWidth="1"/>
-    <col min="10" max="10" width="33.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.83203125" customWidth="1"/>
-    <col min="12" max="12" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" customWidth="1"/>
+    <col min="9" max="9" width="35.453125" customWidth="1"/>
+    <col min="10" max="10" width="33.6328125" customWidth="1"/>
+    <col min="11" max="11" width="29.81640625" customWidth="1"/>
+    <col min="12" max="12" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -679,7 +629,7 @@
         <v>-1</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H2">
         <v>-1</v>
@@ -688,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -702,7 +652,7 @@
         <v>-1</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H3">
         <v>-1</v>
@@ -711,7 +661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -725,7 +675,7 @@
         <v>-1</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H4">
         <v>-1</v>
@@ -734,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -748,7 +698,7 @@
         <v>-1</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H5">
         <v>-1</v>
@@ -757,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -771,7 +721,7 @@
         <v>-1</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -780,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -794,7 +744,7 @@
         <v>-1</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H7">
         <v>-1</v>
@@ -803,7 +753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -817,7 +767,7 @@
         <v>-1</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8">
         <v>-1</v>
@@ -826,7 +776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -840,7 +790,7 @@
         <v>-1</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H9">
         <v>-1</v>
@@ -849,7 +799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -863,7 +813,7 @@
         <v>-1</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10">
         <v>-1</v>
@@ -872,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -886,7 +836,7 @@
         <v>-1</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H11">
         <v>-1</v>
@@ -895,7 +845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -909,7 +859,7 @@
         <v>-1</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12">
         <v>-1</v>
@@ -918,7 +868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -932,7 +882,7 @@
         <v>-1</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -941,7 +891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -955,7 +905,7 @@
         <v>-1</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H14">
         <v>-1</v>
@@ -964,7 +914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -978,7 +928,7 @@
         <v>-1</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>-1</v>
@@ -987,7 +937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1001,7 +951,7 @@
         <v>-1</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H16">
         <v>-1</v>
@@ -1010,7 +960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1024,7 +974,7 @@
         <v>-1</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H17">
         <v>-1</v>
@@ -1033,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1047,7 +997,7 @@
         <v>-1</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H18">
         <v>-1</v>
@@ -1056,7 +1006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1070,7 +1020,7 @@
         <v>-1</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H19">
         <v>-1</v>
@@ -1079,7 +1029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1093,7 +1043,7 @@
         <v>-1</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H20">
         <v>-1</v>
@@ -1102,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1116,7 +1066,7 @@
         <v>-1</v>
       </c>
       <c r="G21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H21">
         <v>-1</v>
@@ -1125,7 +1075,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1089,7 @@
         <v>-1</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H22">
         <v>-1</v>
@@ -1148,7 +1098,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1162,7 +1112,7 @@
         <v>-1</v>
       </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -1171,7 +1121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1185,7 +1135,7 @@
         <v>-1</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H24">
         <v>-1</v>
@@ -1194,7 +1144,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1208,19 +1158,19 @@
         <v>-1</v>
       </c>
       <c r="G25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
       </c>
       <c r="L25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1234,7 +1184,7 @@
         <v>-1</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H26">
         <v>-1</v>
@@ -1243,7 +1193,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1257,7 +1207,7 @@
         <v>-1</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H27">
         <v>-1</v>
@@ -1266,7 +1216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1280,7 +1230,7 @@
         <v>-1</v>
       </c>
       <c r="G28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H28">
         <v>-1</v>
@@ -1289,7 +1239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1303,22 +1253,22 @@
         <v>-1</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I29" t="s">
         <v>29</v>
       </c>
       <c r="J29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1332,19 +1282,19 @@
         <v>-1</v>
       </c>
       <c r="G30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I30" t="s">
         <v>30</v>
       </c>
       <c r="L30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1355,19 +1305,19 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H31">
         <v>-1</v>
       </c>
       <c r="I31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1378,19 +1328,19 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G32" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H32">
         <v>-1</v>
       </c>
       <c r="I32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1404,7 +1354,7 @@
         <v>-1</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H33">
         <v>-1</v>
@@ -1413,7 +1363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1421,13 +1371,13 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D34">
         <v>-1</v>
       </c>
       <c r="G34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H34">
         <v>-1</v>
@@ -1436,7 +1386,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1444,13 +1394,13 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D35">
         <v>-1</v>
       </c>
       <c r="G35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H35">
         <v>-1</v>
@@ -1459,7 +1409,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1473,16 +1423,22 @@
         <v>-1</v>
       </c>
       <c r="G36" t="s">
-        <v>47</v>
-      </c>
-      <c r="H36">
-        <v>-1</v>
+        <v>48</v>
+      </c>
+      <c r="H36" t="s">
+        <v>60</v>
       </c>
       <c r="I36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>59</v>
+      </c>
+      <c r="L36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1490,13 +1446,13 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>-1</v>
       </c>
       <c r="G37" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H37">
         <v>-1</v>
@@ -1505,7 +1461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1513,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>-1</v>
@@ -1527,71 +1483,19 @@
       <c r="I38" t="s">
         <v>38</v>
       </c>
-      <c r="J38" t="s">
-        <v>62</v>
-      </c>
       <c r="L38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>-1</v>
+        <v>54</v>
       </c>
       <c r="G39" t="s">
-        <v>53</v>
-      </c>
-      <c r="H39">
-        <v>-1</v>
+        <v>56</v>
       </c>
       <c r="I39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>-1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>52</v>
-      </c>
-      <c r="H40" t="s">
-        <v>66</v>
-      </c>
-      <c r="I40" t="s">
-        <v>40</v>
-      </c>
-      <c r="L40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>57</v>
-      </c>
-      <c r="G41" t="s">
-        <v>59</v>
-      </c>
-      <c r="I41" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1600,24 +1504,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>